<commit_message>
Add $BA basic model structure, update Aerospace Overview
</commit_message>
<xml_diff>
--- a/$BA.xlsx
+++ b/$BA.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1ED9774-A0CD-4C63-8353-F9DBB415B8ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F93E99-16CF-414C-8385-9AF386070A46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{CFD6F5FA-5FC8-4575-A1DD-3D928AF17DDA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{CFD6F5FA-5FC8-4575-A1DD-3D928AF17DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
-    <sheet name="Financial Model" sheetId="2" r:id="rId2"/>
+    <sheet name="Financial Model" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,9 +25,80 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t>$BA</t>
+  </si>
+  <si>
+    <t>The Boeing Company</t>
+  </si>
+  <si>
+    <t>Stock Snapshot</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Shares</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Debt</t>
+  </si>
+  <si>
+    <t>Net Cash</t>
+  </si>
+  <si>
+    <t>EV</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>CFO</t>
+  </si>
+  <si>
+    <t>COO</t>
+  </si>
+  <si>
+    <t>Chair</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>HQ</t>
+  </si>
+  <si>
+    <t>Founded</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>Key Metrics</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="#,##0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -41,16 +112,48 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -58,13 +161,131 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -80,6 +301,67 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1724026" cy="400701"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="File:Boeing full logo.svg - Wikimedia Commons">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49373175-FE17-4F7F-BFDE-FAE3DB23E235}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2228850" y="152401"/>
+          <a:ext cx="1724026" cy="400701"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -379,6 +661,230 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D03AC0-1305-4B2C-ACAE-AA469A6FF895}">
+  <dimension ref="B2:D37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8">
+        <v>141.32</v>
+      </c>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="24">
+        <v>593.80999999999995</v>
+      </c>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="24">
+        <f>C7*C8</f>
+        <v>83917.229199999987</v>
+      </c>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="24">
+        <f>C10-C11</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="25">
+        <f>C9-C12</f>
+        <v>83917.229199999987</v>
+      </c>
+      <c r="D13" s="11"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="20"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="18"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="20"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="14"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="18"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="20"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="20"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="22"/>
+      <c r="D30" s="23"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="14"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="14"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="14"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565453A5-32EF-4F02-AECB-0C4BFA388139}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -392,21 +898,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36EC1510-860F-4922-980A-5D6E8D6361F5}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>